<commit_message>
Deploying to gh-pages from @ hustliyilin/content@a0ed21c556fc4c0ab15b21a37c6da600cc11a97f 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5 (2),SC-5</t>
+          <t>SC-5,SC-5 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-6 (8),AU-8 b,CM-5 (1),AU-7 b,AU-7 a,AU-12 (3)</t>
+          <t>AU-7 a,AC-6 (8),AC-6 (9),AU-7 b,AU-8 b,CM-5 (1),AU-12 (3)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,CM-6 b,AU-12 a,AU-12 c,CM-5 (1),AU-7 b,AU-8 b,AU-12 (3)</t>
+          <t>AU-7 a,AU-7 b,AU-12 c,AU-8 b,CM-6 b,AU-12 a,CM-5 (1),AU-12 (3)</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,AC-17 (9),CM-7 b</t>
+          <t>AC-17 (9),CM-7 b,CM-6 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -3286,7 +3286,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3370,7 +3370,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3455,7 +3455,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3527,7 +3527,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-8,AU-3 (1),IA-2</t>
+          <t>AU-3 (1),IA-8,IA-2</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3985,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4435,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4510,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4585,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4660,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4735,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4810,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4885,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4965,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5208,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5288,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5664,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5738,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5811,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5957,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6176,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6324,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6398,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6469,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6549,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6629,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6789,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6869,7 +6869,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6949,7 +6949,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7189,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7269,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7349,7 +7349,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7425,7 +7425,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7502,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7982,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8062,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8142,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8222,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8295,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8457,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8528,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8685,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8767,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8849,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9013,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-14 (1),AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-14 (1),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9096,7 +9096,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9177,7 +9177,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9263,7 +9263,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9341,7 +9341,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9707,7 +9707,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9849,7 +9849,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10222,7 +10222,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,CM-5 (1),AC-6 (9)</t>
+          <t>CM-5 (1),AC-2 (4),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10345,7 +10345,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10665,7 +10665,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 c,AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2),SC-13,MA-4 c</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10747,7 +10747,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),MA-4 e,AC-12,SC-10</t>
+          <t>MA-4 (7),MA-4 e,SC-10,AC-12</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10822,7 +10822,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10901,7 +10901,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11054,7 +11054,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1),AU-12 a,AU-14 (1),AU-3 (1),AU-7 (1),MA-4 (1) (a),AU-6 (4),AU-7 a,AU-3</t>
+          <t>AU-6 (4),AU-7 (1),AU-7 a,AU-14 (1),AU-3 (1),CM-6 b,AU-3,AU-12 a,CM-5 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11291,7 +11291,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11367,7 +11367,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -13112,7 +13112,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13265,7 +13265,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13344,7 +13344,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13419,7 +13419,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -13494,7 +13494,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
+          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13708,7 +13708,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13786,7 +13786,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -13869,7 +13869,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -14249,7 +14249,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
+          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14320,7 +14320,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14399,7 +14399,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14471,7 +14471,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14543,7 +14543,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14617,7 +14617,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14691,7 +14691,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14765,7 +14765,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15720,7 +15720,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16315,7 +16315,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17362,7 +17362,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17440,7 +17440,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (5),IA-2 (3),IA-2</t>
+          <t>IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17525,7 +17525,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (5),IA-2 (3),IA-2</t>
+          <t>IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17610,7 +17610,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>SC-8,AC-18 (1),SC-8 (1)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17777,7 +17777,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -17860,7 +17860,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -17936,7 +17936,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18021,7 +18021,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18178,7 +18178,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18257,7 +18257,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -18341,7 +18341,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -18416,7 +18416,7 @@
     <row r="233" ht="130" customHeight="1">
       <c r="A233" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B233" s="2" t="inlineStr">
@@ -19246,7 +19246,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>SC-2,CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -19406,7 +19406,7 @@
     <row r="246" ht="130" customHeight="1">
       <c r="A246" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B246" s="2" t="inlineStr">
@@ -20320,7 +20320,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -20395,7 +20395,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20483,7 +20483,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20560,7 +20560,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -21158,7 +21158,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21245,7 +21245,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (2),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2 (1),IA-2 (4)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21632,7 +21632,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -22039,7 +22039,7 @@
     <row r="280" ht="130" customHeight="1">
       <c r="A280" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B280" s="2" t="inlineStr">
@@ -22262,7 +22262,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -23442,7 +23442,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23531,7 +23531,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24353,7 +24353,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25770,7 +25770,7 @@
     <row r="327" ht="130" customHeight="1">
       <c r="A327" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,CM-5 (1)</t>
+          <t>CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B327" s="2" t="inlineStr">
@@ -25927,7 +25927,7 @@
     <row r="329" ht="130" customHeight="1">
       <c r="A329" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B329" s="2" t="inlineStr">
@@ -26846,7 +26846,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -26921,7 +26921,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -26995,7 +26995,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27069,7 +27069,7 @@
     <row r="344" ht="130" customHeight="1">
       <c r="A344" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B344" s="2" t="inlineStr">
@@ -27155,7 +27155,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27232,7 +27232,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28326,7 +28326,7 @@
     <row r="360" ht="130" customHeight="1">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 b,SI-6 d</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
@@ -28410,7 +28410,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -29330,7 +29330,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29401,7 +29401,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29473,7 +29473,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -30233,7 +30233,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -30542,7 +30542,7 @@
     <row r="388" ht="130" customHeight="1">
       <c r="A388" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B388" s="2" t="inlineStr">
@@ -30912,7 +30912,7 @@
     <row r="393" ht="130" customHeight="1">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
@@ -31237,7 +31237,7 @@
     <row r="397" ht="130" customHeight="1">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
@@ -31328,7 +31328,7 @@
     <row r="398" ht="130" customHeight="1">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
@@ -31422,7 +31422,7 @@
     <row r="399" ht="130" customHeight="1">
       <c r="A399" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B399" s="2" t="inlineStr">
@@ -34832,7 +34832,7 @@
     <row r="444" ht="130" customHeight="1">
       <c r="A444" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B444" s="2" t="inlineStr">
@@ -34982,7 +34982,7 @@
     <row r="446" ht="130" customHeight="1">
       <c r="A446" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B446" s="2" t="inlineStr">
@@ -35055,7 +35055,7 @@
     <row r="447" ht="130" customHeight="1">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
@@ -42185,7 +42185,7 @@
     <row r="537" ht="130" customHeight="1">
       <c r="A537" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B537" s="2" t="inlineStr">
@@ -42832,7 +42832,7 @@
     <row r="546" ht="130" customHeight="1">
       <c r="A546" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B546" s="2" t="inlineStr">
@@ -43428,7 +43428,7 @@
     <row r="554" ht="130" customHeight="1">
       <c r="A554" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B554" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ hustliyilin/content@aff71793662733ea96701c8baf79fdefc881a9b5 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AC-6 (8),AC-6 (9),AU-7 b,AU-8 b,CM-5 (1),AU-12 (3)</t>
+          <t>AU-7 a,AC-6 (9),AC-6 (8),CM-5 (1),AU-7 b,AU-8 b,AU-12 (3)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-7 b,AU-12 c,AU-8 b,CM-6 b,AU-12 a,CM-5 (1),AU-12 (3)</t>
+          <t>CM-6 b,AU-7 a,AU-12 c,CM-5 (1),AU-7 b,AU-8 b,AU-12 (3),AU-12 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (1),AC-17 (9),CM-6 b</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1484,7 +1484,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1560,7 +1560,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1714,7 +1714,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2084,7 +2084,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2158,7 +2158,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3286,7 +3286,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3370,7 +3370,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3455,7 +3455,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3527,7 +3527,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3985,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4435,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4510,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4585,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4660,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4735,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4810,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4885,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4965,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5208,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5288,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5664,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5738,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5811,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5957,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6176,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6324,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6398,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6469,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6549,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6629,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6789,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6869,7 +6869,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6949,7 +6949,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7189,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7269,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7349,7 +7349,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7425,7 +7425,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7502,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7982,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8062,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8142,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8222,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8295,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8457,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8528,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8685,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8767,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8849,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9013,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-3 (1),AU-12 c,AU-3,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-14 (1),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9707,7 +9707,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9849,7 +9849,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10222,7 +10222,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9),CM-5 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10345,7 +10345,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10665,7 +10665,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),SC-13,MA-4 c</t>
+          <t>SC-13,SC-8,AC-17 (2),MA-4 c</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10747,7 +10747,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),MA-4 e,SC-10,AC-12</t>
+          <t>MA-4 (7),MA-4 e,AC-12,SC-10</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10822,7 +10822,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10901,7 +10901,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11054,7 +11054,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-7 (1),AU-7 a,AU-14 (1),AU-3 (1),CM-6 b,AU-3,AU-12 a,CM-5 (1),MA-4 (1) (a)</t>
+          <t>AU-14 (1),AU-6 (4),AU-3 (1),CM-6 b,AU-7 a,CM-5 (1),AU-7 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -13265,7 +13265,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13419,7 +13419,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -13494,7 +13494,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13708,7 +13708,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13786,7 +13786,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -13869,7 +13869,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -14249,7 +14249,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14320,7 +14320,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -15286,7 +15286,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15720,7 +15720,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16235,7 +16235,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16315,7 +16315,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17362,7 +17362,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17440,7 +17440,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4),IA-2</t>
+          <t>IA-2 (5),IA-2 (2),IA-2 (3),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17525,7 +17525,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4),IA-2</t>
+          <t>IA-2 (5),IA-2 (2),IA-2 (3),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17610,7 +17610,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17777,7 +17777,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18178,7 +18178,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18257,7 +18257,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -18416,7 +18416,7 @@
     <row r="233" ht="130" customHeight="1">
       <c r="A233" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B233" s="2" t="inlineStr">
@@ -19246,7 +19246,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -21245,7 +21245,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2 (1),IA-2 (4)</t>
+          <t>IA-2 (4),IA-2 (1),IA-2 (2),IA-2 (3)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21713,7 +21713,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -21801,7 +21801,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22262,7 +22262,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -23442,7 +23442,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23531,7 +23531,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24353,7 +24353,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25770,7 +25770,7 @@
     <row r="327" ht="130" customHeight="1">
       <c r="A327" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c</t>
+          <t>AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B327" s="2" t="inlineStr">
@@ -27155,7 +27155,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27232,7 +27232,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28077,7 +28077,7 @@
     <row r="357" ht="130" customHeight="1">
       <c r="A357" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B357" s="2" t="inlineStr">
@@ -28326,7 +28326,7 @@
     <row r="360" ht="130" customHeight="1">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 b,SI-6 d</t>
+          <t>CM-3 (5),SI-6 d,SI-6 b</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
@@ -28410,7 +28410,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -29330,7 +29330,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29401,7 +29401,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29473,7 +29473,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -30681,7 +30681,7 @@
     <row r="390" ht="130" customHeight="1">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
@@ -30996,7 +30996,7 @@
     <row r="394" ht="130" customHeight="1">
       <c r="A394" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B394" s="2" t="inlineStr">
@@ -34832,7 +34832,7 @@
     <row r="444" ht="130" customHeight="1">
       <c r="A444" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B444" s="2" t="inlineStr">
@@ -40866,7 +40866,7 @@
     <row r="520" ht="130" customHeight="1">
       <c r="A520" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B520" s="2" t="inlineStr">
@@ -40953,7 +40953,7 @@
     <row r="521" ht="130" customHeight="1">
       <c r="A521" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B521" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ hustliyilin/content@9da44b1fe4a95043aaef69c92280f983b233279b 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -710,7 +710,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -782,7 +782,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1446,7 +1446,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-3 (1),AU-12 a,AU-3,AU-7 a,AU-7 (1),AU-14 (1),MA-4 (1) (a),CM-6 b,AU-6 (4)</t>
+          <t>AU-3,AU-14 (1),CM-5 (1),AU-7 (1),CM-6 b,AU-12 a,MA-4 (1) (a),AU-7 a,AU-3 (1),AU-6 (4)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1531,7 +1531,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1607,7 +1607,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1761,7 +1761,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2131,7 +2131,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2205,7 +2205,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3249,7 +3249,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-14 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-14 (1),AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3331,7 +3331,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -4152,7 +4152,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4302,7 +4302,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4457,7 +4457,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4533,7 +4533,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4617,7 +4617,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4693,7 +4693,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5),SI-6 b</t>
+          <t>SI-6 b,CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4778,7 +4778,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4862,7 +4862,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4937,7 +4937,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -5012,7 +5012,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5087,7 +5087,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5162,7 +5162,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5237,7 +5237,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5312,7 +5312,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5387,7 +5387,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5462,7 +5462,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5537,7 +5537,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 a,AU-7 a,AU-8 b,AU-12 c,AU-7 b,AU-12 (3),CM-6 b</t>
+          <t>AU-12 (3),CM-6 b,AU-8 b,AU-12 a,AU-12 c,AU-7 a,AU-7 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -6536,7 +6536,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AC-6 (9),AU-12 c,AC-2 (4),CM-5 (1)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6603,7 +6603,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6684,7 +6684,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6765,7 +6765,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6847,7 +6847,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6929,7 +6929,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -7011,7 +7011,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7093,7 +7093,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7175,7 +7175,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7244,7 +7244,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-6 (9),AU-7 a,AU-8 b,AC-6 (8),AU-7 b,AU-12 (3)</t>
+          <t>AU-12 (3),AC-6 (8),AU-8 b,AC-6 (9),AU-7 a,AU-7 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7324,7 +7324,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7396,7 +7396,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7468,7 +7468,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7542,7 +7542,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7616,7 +7616,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7690,7 +7690,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -8269,7 +8269,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8343,7 +8343,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8417,7 +8417,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8491,7 +8491,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8648,7 +8648,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8733,7 +8733,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8809,7 +8809,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8979,7 +8979,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9055,7 +9055,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9131,7 +9131,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9206,7 +9206,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9281,7 +9281,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9356,7 +9356,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9436,7 +9436,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
@@ -9510,7 +9510,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9584,7 +9584,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9658,7 +9658,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9732,7 +9732,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -9806,7 +9806,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9886,7 +9886,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9966,7 +9966,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -10046,7 +10046,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10117,7 +10117,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10288,7 +10288,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10367,7 +10367,7 @@
     <row r="130" ht="130" customHeight="1">
       <c r="A130" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B130" s="2" t="inlineStr">
@@ -10446,7 +10446,7 @@
     <row r="131" ht="130" customHeight="1">
       <c r="A131" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B131" s="2" t="inlineStr">
@@ -10530,7 +10530,7 @@
     <row r="132" ht="130" customHeight="1">
       <c r="A132" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B132" s="2" t="inlineStr">
@@ -10778,7 +10778,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-13,MA-4 c,SC-8</t>
+          <t>AC-17 (2),MA-4 c,SC-13,SC-8</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10860,7 +10860,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10931,7 +10931,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11002,7 +11002,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11073,7 +11073,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11153,7 +11153,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B140" s="2" t="inlineStr">
@@ -11222,7 +11222,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11291,7 +11291,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -11360,7 +11360,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11429,7 +11429,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -12276,7 +12276,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -12357,7 +12357,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12443,7 +12443,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12809,7 +12809,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B161" s="2" t="inlineStr">
@@ -12889,7 +12889,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
@@ -12969,7 +12969,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B163" s="2" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13361,7 +13361,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -14145,7 +14145,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14222,7 +14222,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14295,7 +14295,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14368,7 +14368,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14453,7 +14453,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14528,7 +14528,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14603,7 +14603,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14678,7 +14678,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14753,7 +14753,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14824,7 +14824,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -14895,7 +14895,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B188" s="2" t="inlineStr">
@@ -14967,7 +14967,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B189" s="2" t="inlineStr">
@@ -15038,7 +15038,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B190" s="2" t="inlineStr">
@@ -15109,7 +15109,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B191" s="2" t="inlineStr">
@@ -15181,7 +15181,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15256,7 +15256,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15327,7 +15327,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15398,7 +15398,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B195" s="2" t="inlineStr">
@@ -15470,7 +15470,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15545,7 +15545,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15627,7 +15627,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15709,7 +15709,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -15791,7 +15791,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -15873,7 +15873,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -15955,7 +15955,7 @@
     <row r="202" ht="130" customHeight="1">
       <c r="A202" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B202" s="2" t="inlineStr">
@@ -16037,7 +16037,7 @@
     <row r="203" ht="130" customHeight="1">
       <c r="A203" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B203" s="2" t="inlineStr">
@@ -16119,7 +16119,7 @@
     <row r="204" ht="130" customHeight="1">
       <c r="A204" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B204" s="2" t="inlineStr">
@@ -16201,7 +16201,7 @@
     <row r="205" ht="130" customHeight="1">
       <c r="A205" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B205" s="2" t="inlineStr">
@@ -16283,7 +16283,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16361,7 +16361,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16440,7 +16440,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16522,7 +16522,7 @@
     <row r="209" ht="130" customHeight="1">
       <c r="A209" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B209" s="2" t="inlineStr">
@@ -16604,7 +16604,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16686,7 +16686,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16768,7 +16768,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16850,7 +16850,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -16932,7 +16932,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17007,7 +17007,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17084,7 +17084,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (2),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (4),IA-2 (2),IA-2 (3)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17171,7 +17171,7 @@
     <row r="217" ht="130" customHeight="1">
       <c r="A217" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2,IA-2 (4),IA-2 (3),IA-2 (5)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2,IA-2 (5)</t>
         </is>
       </c>
       <c r="B217" s="2" t="inlineStr">
@@ -17260,7 +17260,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2,IA-2 (4),IA-2 (3),IA-2 (5)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2,IA-2 (5)</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -17498,7 +17498,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -18000,7 +18000,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-18 (1)</t>
+          <t>SC-8,AC-18 (1),SC-8 (1)</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18928,7 +18928,7 @@
     <row r="240" ht="130" customHeight="1">
       <c r="A240" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B240" s="2" t="inlineStr">
@@ -19014,7 +19014,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),CM-6 b,SC-5</t>
+          <t>SC-5,SC-5 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19194,7 +19194,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -19277,7 +19277,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -20342,7 +20342,7 @@
     <row r="257" ht="130" customHeight="1">
       <c r="A257" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b,SI-16</t>
+          <t>SI-16,SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B257" s="2" t="inlineStr">
@@ -20502,7 +20502,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-16</t>
+          <t>SI-16,SC-3</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -21187,7 +21187,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -22011,7 +22011,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -22100,7 +22100,7 @@
     <row r="279" ht="130" customHeight="1">
       <c r="A279" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B279" s="2" t="inlineStr">
@@ -22585,7 +22585,7 @@
     <row r="285" ht="130" customHeight="1">
       <c r="A285" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B285" s="2" t="inlineStr">
@@ -23087,7 +23087,7 @@
     <row r="291" ht="130" customHeight="1">
       <c r="A291" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B291" s="2" t="inlineStr">
@@ -31217,7 +31217,7 @@
     <row r="399" ht="130" customHeight="1">
       <c r="A399" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B399" s="2" t="inlineStr">
@@ -31855,7 +31855,7 @@
     <row r="407" ht="130" customHeight="1">
       <c r="A407" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (9),CM-6 b,AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (9),AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B407" s="2" t="inlineStr">
@@ -31933,7 +31933,7 @@
     <row r="408" ht="130" customHeight="1">
       <c r="A408" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B408" s="2" t="inlineStr">
@@ -37008,7 +37008,7 @@
     <row r="470" ht="130" customHeight="1">
       <c r="A470" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B470" s="2" t="inlineStr">
@@ -37655,7 +37655,7 @@
     <row r="479" ht="130" customHeight="1">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
@@ -37946,7 +37946,7 @@
     <row r="483" ht="130" customHeight="1">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,AC-12,SC-10,MA-4 (7)</t>
+          <t>MA-4 e,AC-12,MA-4 (7),SC-10</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ hustliyilin/content@414e8c1f55037f3b3931e7ec682b2e9aa980a9b0 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -1446,7 +1446,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-14 (1),CM-5 (1),AU-7 (1),CM-6 b,AU-12 a,MA-4 (1) (a),AU-7 a,AU-3 (1),AU-6 (4)</t>
+          <t>AU-14 (1),AU-7 a,MA-4 (1) (a),AU-3 (1),CM-5 (1),AU-7 (1),CM-6 b,AU-3,AU-6 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -3249,7 +3249,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-14 (1),AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3773,7 +3773,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -4152,7 +4152,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
+          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4302,7 +4302,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4457,7 +4457,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4533,7 +4533,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4617,7 +4617,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4862,7 +4862,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4937,7 +4937,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -5012,7 +5012,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5087,7 +5087,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5162,7 +5162,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5237,7 +5237,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5312,7 +5312,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5387,7 +5387,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5462,7 +5462,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5537,7 +5537,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),CM-6 b,AU-8 b,AU-12 a,AU-12 c,AU-7 a,AU-7 b,CM-5 (1)</t>
+          <t>AU-12 (3),AU-7 b,CM-5 (1),CM-6 b,AU-8 b,AU-7 a,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -6536,7 +6536,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 c,AC-2 (4),CM-5 (1)</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9),CM-5 (1)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6603,7 +6603,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6684,7 +6684,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6765,7 +6765,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6847,7 +6847,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6929,7 +6929,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -7011,7 +7011,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7093,7 +7093,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7175,7 +7175,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7244,7 +7244,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AC-6 (8),AU-8 b,AC-6 (9),AU-7 a,AU-7 b,CM-5 (1)</t>
+          <t>AU-12 (3),AC-6 (8),AU-7 b,CM-5 (1),AU-8 b,AU-7 a,AC-6 (9)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -8269,7 +8269,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8343,7 +8343,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8417,7 +8417,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8491,7 +8491,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8648,7 +8648,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8809,7 +8809,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8979,7 +8979,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9055,7 +9055,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9131,7 +9131,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9206,7 +9206,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9281,7 +9281,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9356,7 +9356,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9436,7 +9436,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
@@ -9510,7 +9510,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9584,7 +9584,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9658,7 +9658,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9732,7 +9732,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -9806,7 +9806,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9886,7 +9886,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9966,7 +9966,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -10046,7 +10046,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10117,7 +10117,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10367,7 +10367,7 @@
     <row r="130" ht="130" customHeight="1">
       <c r="A130" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B130" s="2" t="inlineStr">
@@ -10446,7 +10446,7 @@
     <row r="131" ht="130" customHeight="1">
       <c r="A131" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B131" s="2" t="inlineStr">
@@ -10530,7 +10530,7 @@
     <row r="132" ht="130" customHeight="1">
       <c r="A132" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B132" s="2" t="inlineStr">
@@ -10778,7 +10778,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 c,SC-13,SC-8</t>
+          <t>AC-17 (2),SC-13,MA-4 c,SC-8</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10931,7 +10931,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11073,7 +11073,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11429,7 +11429,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11509,7 +11509,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -12889,7 +12889,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
@@ -12969,7 +12969,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B163" s="2" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13748,7 +13748,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13824,7 +13824,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -13909,7 +13909,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -14066,7 +14066,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B177" s="2" t="inlineStr">
@@ -14145,7 +14145,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14222,7 +14222,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14295,7 +14295,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14368,7 +14368,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14453,7 +14453,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14528,7 +14528,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14603,7 +14603,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14678,7 +14678,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -15181,7 +15181,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15470,7 +15470,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15545,7 +15545,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15627,7 +15627,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15709,7 +15709,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -15791,7 +15791,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -15873,7 +15873,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -15955,7 +15955,7 @@
     <row r="202" ht="130" customHeight="1">
       <c r="A202" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B202" s="2" t="inlineStr">
@@ -16037,7 +16037,7 @@
     <row r="203" ht="130" customHeight="1">
       <c r="A203" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B203" s="2" t="inlineStr">
@@ -16119,7 +16119,7 @@
     <row r="204" ht="130" customHeight="1">
       <c r="A204" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B204" s="2" t="inlineStr">
@@ -16201,7 +16201,7 @@
     <row r="205" ht="130" customHeight="1">
       <c r="A205" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B205" s="2" t="inlineStr">
@@ -16283,7 +16283,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16361,7 +16361,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16440,7 +16440,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16522,7 +16522,7 @@
     <row r="209" ht="130" customHeight="1">
       <c r="A209" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B209" s="2" t="inlineStr">
@@ -16604,7 +16604,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16686,7 +16686,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16768,7 +16768,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16850,7 +16850,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -16932,7 +16932,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17007,7 +17007,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17084,7 +17084,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (4),IA-2 (2),IA-2 (3)</t>
+          <t>IA-2 (1),IA-2 (3),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17171,7 +17171,7 @@
     <row r="217" ht="130" customHeight="1">
       <c r="A217" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2,IA-2 (5)</t>
+          <t>IA-2 (5),IA-2 (4),IA-2 (3),IA-2,IA-2 (2)</t>
         </is>
       </c>
       <c r="B217" s="2" t="inlineStr">
@@ -17260,7 +17260,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2,IA-2 (5)</t>
+          <t>IA-2 (5),IA-2 (4),IA-2 (3),IA-2,IA-2 (2)</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -17928,7 +17928,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18000,7 +18000,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18160,7 +18160,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18768,7 +18768,7 @@
     <row r="238" ht="130" customHeight="1">
       <c r="A238" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B238" s="2" t="inlineStr">
@@ -19014,7 +19014,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>SC-5 (2),CM-6 b,SC-5</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19194,7 +19194,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -19368,7 +19368,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -20342,7 +20342,7 @@
     <row r="257" ht="130" customHeight="1">
       <c r="A257" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-2,CM-6 b</t>
+          <t>SC-2,SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B257" s="2" t="inlineStr">
@@ -21187,7 +21187,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -21836,7 +21836,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -21924,7 +21924,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22100,7 +22100,7 @@
     <row r="279" ht="130" customHeight="1">
       <c r="A279" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B279" s="2" t="inlineStr">
@@ -22585,7 +22585,7 @@
     <row r="285" ht="130" customHeight="1">
       <c r="A285" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
         </is>
       </c>
       <c r="B285" s="2" t="inlineStr">
@@ -23087,7 +23087,7 @@
     <row r="291" ht="130" customHeight="1">
       <c r="A291" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B291" s="2" t="inlineStr">
@@ -23650,7 +23650,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -25089,7 +25089,7 @@
     <row r="317" ht="130" customHeight="1">
       <c r="A317" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c</t>
+          <t>AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B317" s="2" t="inlineStr">
@@ -28607,7 +28607,7 @@
     <row r="364" ht="130" customHeight="1">
       <c r="A364" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B364" s="2" t="inlineStr">
@@ -28757,7 +28757,7 @@
     <row r="366" ht="130" customHeight="1">
       <c r="A366" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B366" s="2" t="inlineStr">
@@ -28837,7 +28837,7 @@
     <row r="367" ht="130" customHeight="1">
       <c r="A367" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B367" s="2" t="inlineStr">
@@ -28910,7 +28910,7 @@
     <row r="368" ht="130" customHeight="1">
       <c r="A368" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B368" s="2" t="inlineStr">
@@ -31461,7 +31461,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -31855,7 +31855,7 @@
     <row r="407" ht="130" customHeight="1">
       <c r="A407" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (9),AC-17 (1),CM-6 b</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b,AC-17 (9)</t>
         </is>
       </c>
       <c r="B407" s="2" t="inlineStr">
@@ -35194,7 +35194,7 @@
     <row r="447" ht="130" customHeight="1">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
@@ -35797,7 +35797,7 @@
     <row r="454" ht="130" customHeight="1">
       <c r="A454" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B454" s="2" t="inlineStr">
@@ -36249,7 +36249,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B460" s="2" t="inlineStr">
@@ -37946,7 +37946,7 @@
     <row r="483" ht="130" customHeight="1">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,AC-12,MA-4 (7),SC-10</t>
+          <t>SC-10,AC-12,MA-4 e,MA-4 (7)</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">
@@ -38021,7 +38021,7 @@
     <row r="484" ht="130" customHeight="1">
       <c r="A484" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B484" s="2" t="inlineStr">
@@ -38100,7 +38100,7 @@
     <row r="485" ht="130" customHeight="1">
       <c r="A485" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B485" s="2" t="inlineStr">
@@ -38176,7 +38176,7 @@
     <row r="486" ht="130" customHeight="1">
       <c r="A486" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B486" s="2" t="inlineStr">
@@ -41011,7 +41011,7 @@
     <row r="523" ht="130" customHeight="1">
       <c r="A523" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B523" s="2" t="inlineStr">
@@ -41113,7 +41113,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -41223,7 +41223,7 @@
     <row r="525" ht="130" customHeight="1">
       <c r="A525" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B525" s="2" t="inlineStr">
@@ -41334,7 +41334,7 @@
     <row r="526" ht="130" customHeight="1">
       <c r="A526" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B526" s="2" t="inlineStr">
@@ -42037,7 +42037,7 @@
     <row r="535" ht="130" customHeight="1">
       <c r="A535" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B535" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ hustliyilin/content@c6b161d440add9263eb8abd80fe1e1883d3224d5 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -964,7 +964,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1446,7 +1446,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-7 a,MA-4 (1) (a),AU-3 (1),CM-5 (1),AU-7 (1),CM-6 b,AU-3,AU-6 (4),AU-12 a</t>
+          <t>AU-6 (4),AU-7 a,MA-4 (1) (a),AU-7 (1),CM-5 (1),AU-3 (1),AU-3,CM-6 b,AU-14 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -3249,7 +3249,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-14 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3331,7 +3331,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3773,7 +3773,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -4152,7 +4152,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
+          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4302,7 +4302,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4457,7 +4457,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4533,7 +4533,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4617,7 +4617,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4693,7 +4693,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4778,7 +4778,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4862,7 +4862,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4937,7 +4937,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -5012,7 +5012,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5087,7 +5087,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5162,7 +5162,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5237,7 +5237,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5312,7 +5312,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5387,7 +5387,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5462,7 +5462,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5537,7 +5537,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AU-7 b,CM-5 (1),CM-6 b,AU-8 b,AU-7 a,AU-12 c,AU-12 a</t>
+          <t>AU-8 b,AU-7 a,AU-12 c,AU-12 (3),CM-5 (1),CM-6 b,AU-7 b,AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -6536,7 +6536,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AC-6 (9),CM-5 (1)</t>
+          <t>AC-2 (4),AC-6 (9),AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6603,7 +6603,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6684,7 +6684,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6765,7 +6765,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6847,7 +6847,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6929,7 +6929,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -7011,7 +7011,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7093,7 +7093,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7244,7 +7244,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AC-6 (8),AU-7 b,CM-5 (1),AU-8 b,AU-7 a,AC-6 (9)</t>
+          <t>AU-8 b,AU-7 a,AU-12 (3),CM-5 (1),AC-6 (8),AC-6 (9),AU-7 b</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7324,7 +7324,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7396,7 +7396,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7468,7 +7468,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7542,7 +7542,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7616,7 +7616,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7690,7 +7690,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -8269,7 +8269,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8343,7 +8343,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8417,7 +8417,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8491,7 +8491,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8733,7 +8733,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9131,7 +9131,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9206,7 +9206,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9281,7 +9281,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9356,7 +9356,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9436,7 +9436,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
@@ -9510,7 +9510,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9584,7 +9584,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9658,7 +9658,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9732,7 +9732,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -9806,7 +9806,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9886,7 +9886,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9966,7 +9966,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -10046,7 +10046,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10778,7 +10778,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-13,MA-4 c,SC-8</t>
+          <t>SC-8,AC-17 (2),MA-4 c,SC-13</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10931,7 +10931,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11073,7 +11073,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11429,7 +11429,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11509,7 +11509,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -12889,7 +12889,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
@@ -12969,7 +12969,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B163" s="2" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13361,7 +13361,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13748,7 +13748,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13824,7 +13824,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -13909,7 +13909,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -14066,7 +14066,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B177" s="2" t="inlineStr">
@@ -14145,7 +14145,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14222,7 +14222,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14295,7 +14295,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14368,7 +14368,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14453,7 +14453,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14528,7 +14528,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14603,7 +14603,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14678,7 +14678,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -15181,7 +15181,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15470,7 +15470,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15545,7 +15545,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15627,7 +15627,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15709,7 +15709,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -15791,7 +15791,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -15873,7 +15873,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -15955,7 +15955,7 @@
     <row r="202" ht="130" customHeight="1">
       <c r="A202" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B202" s="2" t="inlineStr">
@@ -16037,7 +16037,7 @@
     <row r="203" ht="130" customHeight="1">
       <c r="A203" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B203" s="2" t="inlineStr">
@@ -16119,7 +16119,7 @@
     <row r="204" ht="130" customHeight="1">
       <c r="A204" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B204" s="2" t="inlineStr">
@@ -16201,7 +16201,7 @@
     <row r="205" ht="130" customHeight="1">
       <c r="A205" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B205" s="2" t="inlineStr">
@@ -16283,7 +16283,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16361,7 +16361,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16440,7 +16440,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16522,7 +16522,7 @@
     <row r="209" ht="130" customHeight="1">
       <c r="A209" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B209" s="2" t="inlineStr">
@@ -16604,7 +16604,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16686,7 +16686,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16768,7 +16768,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16850,7 +16850,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -16932,7 +16932,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17007,7 +17007,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c</t>
+          <t>AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17084,7 +17084,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (3),IA-2 (2),IA-2 (4)</t>
+          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17171,7 +17171,7 @@
     <row r="217" ht="130" customHeight="1">
       <c r="A217" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (4),IA-2 (3),IA-2,IA-2 (2)</t>
+          <t>IA-2 (2),IA-2 (5),IA-2 (3),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B217" s="2" t="inlineStr">
@@ -17260,7 +17260,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (4),IA-2 (3),IA-2,IA-2 (2)</t>
+          <t>IA-2 (2),IA-2 (5),IA-2 (3),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -17928,7 +17928,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18000,7 +18000,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18160,7 +18160,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18768,7 +18768,7 @@
     <row r="238" ht="130" customHeight="1">
       <c r="A238" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B238" s="2" t="inlineStr">
@@ -19014,7 +19014,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),CM-6 b,SC-5</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19277,7 +19277,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -19368,7 +19368,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -20342,7 +20342,7 @@
     <row r="257" ht="130" customHeight="1">
       <c r="A257" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>SC-2,CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B257" s="2" t="inlineStr">
@@ -20502,7 +20502,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -21187,7 +21187,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -21755,7 +21755,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -22100,7 +22100,7 @@
     <row r="279" ht="130" customHeight="1">
       <c r="A279" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B279" s="2" t="inlineStr">
@@ -22425,7 +22425,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -22585,7 +22585,7 @@
     <row r="285" ht="130" customHeight="1">
       <c r="A285" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
+          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B285" s="2" t="inlineStr">
@@ -23087,7 +23087,7 @@
     <row r="291" ht="130" customHeight="1">
       <c r="A291" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B291" s="2" t="inlineStr">
@@ -23952,7 +23952,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B302" s="2" t="inlineStr">
@@ -24026,7 +24026,7 @@
     <row r="303" ht="130" customHeight="1">
       <c r="A303" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B303" s="2" t="inlineStr">
@@ -25245,7 +25245,7 @@
     <row r="319" ht="130" customHeight="1">
       <c r="A319" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B319" s="2" t="inlineStr">
@@ -28607,7 +28607,7 @@
     <row r="364" ht="130" customHeight="1">
       <c r="A364" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B364" s="2" t="inlineStr">
@@ -31217,7 +31217,7 @@
     <row r="399" ht="130" customHeight="1">
       <c r="A399" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B399" s="2" t="inlineStr">
@@ -31461,7 +31461,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -31855,7 +31855,7 @@
     <row r="407" ht="130" customHeight="1">
       <c r="A407" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b,AC-17 (9)</t>
+          <t>AC-17 (1),CM-6 b,AC-17 (9),CM-7 b</t>
         </is>
       </c>
       <c r="B407" s="2" t="inlineStr">
@@ -31933,7 +31933,7 @@
     <row r="408" ht="130" customHeight="1">
       <c r="A408" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B408" s="2" t="inlineStr">
@@ -35194,7 +35194,7 @@
     <row r="447" ht="130" customHeight="1">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
@@ -35797,7 +35797,7 @@
     <row r="454" ht="130" customHeight="1">
       <c r="A454" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B454" s="2" t="inlineStr">
@@ -36249,7 +36249,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B460" s="2" t="inlineStr">
@@ -37946,7 +37946,7 @@
     <row r="483" ht="130" customHeight="1">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12,MA-4 e,MA-4 (7)</t>
+          <t>AC-12,MA-4 (7),MA-4 e,SC-10</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">
@@ -38021,7 +38021,7 @@
     <row r="484" ht="130" customHeight="1">
       <c r="A484" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B484" s="2" t="inlineStr">
@@ -38100,7 +38100,7 @@
     <row r="485" ht="130" customHeight="1">
       <c r="A485" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B485" s="2" t="inlineStr">
@@ -38176,7 +38176,7 @@
     <row r="486" ht="130" customHeight="1">
       <c r="A486" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B486" s="2" t="inlineStr">
@@ -39459,7 +39459,7 @@
     <row r="503" ht="130" customHeight="1">
       <c r="A503" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B503" s="2" t="inlineStr">
@@ -39749,7 +39749,7 @@
     <row r="507" ht="130" customHeight="1">
       <c r="A507" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B507" s="2" t="inlineStr">
@@ -40772,7 +40772,7 @@
     <row r="520" ht="130" customHeight="1">
       <c r="A520" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B520" s="2" t="inlineStr">
@@ -41011,7 +41011,7 @@
     <row r="523" ht="130" customHeight="1">
       <c r="A523" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B523" s="2" t="inlineStr">
@@ -41113,7 +41113,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -41223,7 +41223,7 @@
     <row r="525" ht="130" customHeight="1">
       <c r="A525" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B525" s="2" t="inlineStr">
@@ -41334,7 +41334,7 @@
     <row r="526" ht="130" customHeight="1">
       <c r="A526" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B526" s="2" t="inlineStr">

</xml_diff>